<commit_message>
Fixed Bugs, Modified the validation of the sample, Reorganized files and added files
</commit_message>
<xml_diff>
--- a/Scrappy/Dowloads/output.xlsx
+++ b/Scrappy/Dowloads/output.xlsx
@@ -789,17 +789,17 @@
       </c>
       <c r="B2" s="23" t="inlineStr">
         <is>
-          <t>Cresco Labs, by Heco</t>
+          <t>Contactez-Nous | Cryolor</t>
         </is>
       </c>
       <c r="C2" s="10" t="inlineStr">
         <is>
-          <t>https://www.helloheco.com/project/cresco-labs</t>
+          <t>https://www.cryolor.com/fr/contactez-nous</t>
         </is>
       </c>
       <c r="D2" s="17" t="inlineStr">
         <is>
-          <t>Images(s)</t>
+          <t>contact</t>
         </is>
       </c>
       <c r="E2" s="4" t="inlineStr">
@@ -851,17 +851,17 @@
       </c>
       <c r="B3" s="24" t="inlineStr">
         <is>
-          <t>ōLiv, by Heco</t>
+          <t>Plan du site | Cryolor</t>
         </is>
       </c>
       <c r="C3" s="10" t="inlineStr">
         <is>
-          <t>https://www.helloheco.com/project/oliv</t>
+          <t>https://www.cryolor.com/fr/plan-du-site</t>
         </is>
       </c>
       <c r="D3" s="18" t="inlineStr">
         <is>
-          <t>Images(s)</t>
+          <t>sitemap</t>
         </is>
       </c>
       <c r="E3" s="4" t="inlineStr">
@@ -907,17 +907,17 @@
       </c>
       <c r="B4" s="24" t="inlineStr">
         <is>
-          <t>Blueboard, by Heco</t>
+          <t>Déclaration d’accessibilité Air Liquide Cryolor | Cryolor</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>https://www.helloheco.com/project/blueboard</t>
+          <t>https://www.cryolor.com/fr/accessibilite</t>
         </is>
       </c>
       <c r="D4" s="18" t="inlineStr">
         <is>
-          <t>Images(s), Citation(s)</t>
+          <t>accessibility</t>
         </is>
       </c>
       <c r="E4" s="4" t="inlineStr">
@@ -963,17 +963,13 @@
       </c>
       <c r="B5" s="24" t="inlineStr">
         <is>
-          <t>OnCorps, by Heco</t>
-        </is>
-      </c>
-      <c r="C5" s="10" t="inlineStr">
-        <is>
-          <t>https://www.helloheco.com/project/oncorps</t>
-        </is>
-      </c>
+          <t>Aide</t>
+        </is>
+      </c>
+      <c r="C5" s="10" t="n"/>
       <c r="D5" s="18" t="inlineStr">
         <is>
-          <t>Images(s), Citation(s)</t>
+          <t>Page obligatoire</t>
         </is>
       </c>
       <c r="E5" s="4" t="inlineStr">
@@ -1019,17 +1015,13 @@
       </c>
       <c r="B6" s="24" t="inlineStr">
         <is>
-          <t>west elm Hotels, by Heco</t>
-        </is>
-      </c>
-      <c r="C6" s="10" t="inlineStr">
-        <is>
-          <t>https://www.helloheco.com/project/west-elm-hotels</t>
-        </is>
-      </c>
+          <t>Authentification</t>
+        </is>
+      </c>
+      <c r="C6" s="10" t="n"/>
       <c r="D6" s="18" t="inlineStr">
         <is>
-          <t>Images(s)</t>
+          <t>Page obligatoire</t>
         </is>
       </c>
       <c r="E6" s="4" t="inlineStr">
@@ -1075,17 +1067,13 @@
       </c>
       <c r="B7" s="24" t="inlineStr">
         <is>
-          <t>Bluecrew, by Heco</t>
-        </is>
-      </c>
-      <c r="C7" s="10" t="inlineStr">
-        <is>
-          <t>https://www.helloheco.com/project/bluecrew</t>
-        </is>
-      </c>
+          <t xml:space="preserve">Plan du site </t>
+        </is>
+      </c>
+      <c r="C7" s="10" t="n"/>
       <c r="D7" s="18" t="inlineStr">
         <is>
-          <t>Images(s), Citation(s)</t>
+          <t>Page obligatoire</t>
         </is>
       </c>
       <c r="E7" s="4" t="inlineStr">
@@ -1131,17 +1119,13 @@
       </c>
       <c r="B8" s="24" t="inlineStr">
         <is>
-          <t>Hub on Campus, by Heco</t>
-        </is>
-      </c>
-      <c r="C8" s="10" t="inlineStr">
-        <is>
-          <t>https://www.helloheco.com/project/hub-on-campus</t>
-        </is>
-      </c>
+          <t>Accessibilité</t>
+        </is>
+      </c>
+      <c r="C8" s="10" t="n"/>
       <c r="D8" s="18" t="inlineStr">
         <is>
-          <t>Images(s), Citation(s)</t>
+          <t>Page obligatoire</t>
         </is>
       </c>
       <c r="E8" s="4" t="inlineStr">

</xml_diff>